<commit_message>
fixed the A* problem
</commit_message>
<xml_diff>
--- a/q_16_3_table.xlsx
+++ b/q_16_3_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manor\Desktop\University\Semester6\IntroArtificialInt\hw\ai_hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47B0E9A6-4299-4757-9E2F-B5295237FFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791943A0-D054-4AED-81EA-4B5C02C2E8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F197D31B-EDCC-4A3D-BBFB-E3B3E2A5E2AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F197D31B-EDCC-4A3D-BBFB-E3B3E2A5E2AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,6 +338,72 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,73 +413,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,7 +733,7 @@
   <dimension ref="G1:P30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -750,22 +750,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:16" x14ac:dyDescent="0.2">
-      <c r="G1" s="1">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1">
+      <c r="G1" s="23">
+        <v>8</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23">
         <v>6</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23">
         <v>4</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1">
+      <c r="L1" s="23"/>
+      <c r="M1" s="23">
         <v>2</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="23"/>
       <c r="O1" t="s">
         <v>4</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="O4" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="23">
         <v>0</v>
       </c>
     </row>
@@ -867,7 +867,7 @@
       <c r="O5" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G6">
@@ -897,7 +897,7 @@
       <c r="O6" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="23">
         <v>1</v>
       </c>
     </row>
@@ -929,7 +929,7 @@
       <c r="O7" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="23"/>
     </row>
     <row r="8" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G8">
@@ -959,7 +959,7 @@
       <c r="O8" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="23">
         <v>2</v>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="O9" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G10">
@@ -1021,7 +1021,7 @@
       <c r="O10" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="23">
         <v>3</v>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       <c r="O11" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="23"/>
     </row>
     <row r="12" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G12">
@@ -1083,7 +1083,7 @@
       <c r="O12" t="s">
         <v>1</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="23">
         <v>4</v>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       <c r="O13" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="1"/>
+      <c r="P13" s="23"/>
     </row>
     <row r="14" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G14">
@@ -1145,7 +1145,7 @@
       <c r="O14" t="s">
         <v>1</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="23">
         <v>5</v>
       </c>
     </row>
@@ -1177,316 +1177,311 @@
       <c r="O15" t="s">
         <v>2</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="23"/>
     </row>
     <row r="16" spans="7:16" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="17" t="s">
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O17" s="19" t="s">
+      <c r="O17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="P17" s="23"/>
+      <c r="P17" s="17"/>
     </row>
     <row r="18" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J18" s="5">
-        <v>8</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="J18" s="2">
+        <v>8</v>
+      </c>
+      <c r="K18" s="3">
         <v>6</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="3">
         <v>4</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="4">
         <v>2</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="20" t="s">
+      <c r="N18" s="20"/>
+      <c r="O18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="P18" s="24" t="s">
+      <c r="P18" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J19" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M19" s="13">
+      <c r="J19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="9">
         <v>36</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="13">
         <v>36</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O19" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="8">
+      <c r="J20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="4">
         <v>24</v>
       </c>
-      <c r="N20" s="20">
+      <c r="N20" s="14">
         <v>35</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P20" s="18"/>
+      <c r="P20" s="20"/>
     </row>
     <row r="21" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="12">
+      <c r="J21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="8">
         <v>47</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="15">
         <v>47</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="O21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="P21" s="25">
+      <c r="P21" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J22" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" s="16">
+      <c r="J22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="12">
         <v>49</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="16">
         <v>199</v>
       </c>
-      <c r="O22" s="22" t="s">
+      <c r="O22" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="P22" s="26"/>
+      <c r="P22" s="22"/>
     </row>
     <row r="23" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J23" s="9">
+      <c r="J23" s="5">
         <v>216</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="1">
         <v>216</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="1">
         <v>216</v>
       </c>
-      <c r="M23" s="13">
+      <c r="M23" s="9">
         <v>216</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="13">
         <v>216</v>
       </c>
-      <c r="O23" s="19" t="s">
+      <c r="O23" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P23" s="17">
+      <c r="P23" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J24" s="5">
+      <c r="J24" s="2">
         <v>979</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="3">
         <v>891</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="3">
         <v>468</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="4">
         <v>409</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="14">
         <v>1169</v>
       </c>
-      <c r="O24" s="20" t="s">
+      <c r="O24" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="18"/>
+      <c r="P24" s="20"/>
     </row>
     <row r="25" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J25" s="10">
+      <c r="J25" s="6">
         <v>84</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="7">
         <v>84</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="7">
         <v>84</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="8">
         <v>84</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="15">
         <v>84</v>
       </c>
-      <c r="O25" s="21" t="s">
+      <c r="O25" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="P25" s="25">
+      <c r="P25" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="14">
+      <c r="J26" s="10">
         <v>1606</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="11">
         <v>1383</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="11">
         <v>1159</v>
       </c>
-      <c r="M26" s="16">
+      <c r="M26" s="12">
         <v>340</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="16">
         <v>2287</v>
       </c>
-      <c r="O26" s="22" t="s">
+      <c r="O26" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="P26" s="26"/>
+      <c r="P26" s="22"/>
     </row>
     <row r="27" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J27" s="9">
+      <c r="J27" s="5">
         <v>123</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="1">
         <v>123</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="1">
         <v>123</v>
       </c>
-      <c r="M27" s="13">
+      <c r="M27" s="9">
         <v>123</v>
       </c>
-      <c r="N27" s="19">
+      <c r="N27" s="13">
         <v>123</v>
       </c>
-      <c r="O27" s="19" t="s">
+      <c r="O27" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P27" s="17">
+      <c r="P27" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="5">
+      <c r="J28" s="2">
         <v>137</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="3">
         <v>137</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L28" s="3">
         <v>107</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="4">
         <v>107</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="14">
         <v>743</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P28" s="18"/>
+      <c r="P28" s="20"/>
     </row>
     <row r="29" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="J29" s="10">
+      <c r="J29" s="6">
         <v>367</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="7">
         <v>376</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="7">
         <v>376</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="8">
         <v>376</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="15">
         <v>376</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="P29" s="25">
+      <c r="P29" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="5">
+      <c r="J30" s="2">
         <v>5015</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="3">
         <v>4882</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L30" s="3">
         <v>4530</v>
       </c>
-      <c r="M30" s="8">
+      <c r="M30" s="4">
         <v>3639</v>
       </c>
-      <c r="N30" s="20">
-        <v>5208</v>
-      </c>
-      <c r="O30" s="20" t="s">
+      <c r="N30" s="14">
+        <v>5203</v>
+      </c>
+      <c r="O30" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P30" s="18"/>
+      <c r="P30" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="P27:P28"/>
     <mergeCell ref="P29:P30"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
@@ -1500,6 +1495,11 @@
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="P12:P13"/>
     <mergeCell ref="P14:P15"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="P27:P28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>